<commit_message>
Final version for a fully tied interface and a interface with frictionless sliding. 05/24/2010
</commit_message>
<xml_diff>
--- a/error_computation/frictionless_sliding_analyt_8/database.xlsx
+++ b/error_computation/frictionless_sliding_analyt_8/database.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -486,11 +485,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73883648"/>
-        <c:axId val="73885184"/>
+        <c:axId val="87243008"/>
+        <c:axId val="87248896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73883648"/>
+        <c:axId val="87243008"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -498,12 +497,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73885184"/>
+        <c:crossAx val="87248896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73885184"/>
+        <c:axId val="87248896"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -512,7 +511,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73883648"/>
+        <c:crossAx val="87243008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -525,7 +524,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -852,11 +851,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73903104"/>
-        <c:axId val="73802496"/>
+        <c:axId val="87498752"/>
+        <c:axId val="87500288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73903104"/>
+        <c:axId val="87498752"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -864,12 +863,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73802496"/>
+        <c:crossAx val="87500288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73802496"/>
+        <c:axId val="87500288"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -878,7 +877,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73903104"/>
+        <c:crossAx val="87498752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -891,7 +890,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1232,11 +1231,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73836416"/>
-        <c:axId val="73837952"/>
+        <c:axId val="87553152"/>
+        <c:axId val="87554688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73836416"/>
+        <c:axId val="87553152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1244,12 +1243,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73837952"/>
+        <c:crossAx val="87554688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73837952"/>
+        <c:axId val="87554688"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1258,7 +1257,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73836416"/>
+        <c:crossAx val="87553152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1271,7 +1270,810 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Displacement-norm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lagrange</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$6,Tabelle1!$C$8,Tabelle1!$C$10:$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$G$6,Tabelle1!$G$8,Tabelle1!$G$10:$G$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.15190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3575000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3542999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7796000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5011000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6101000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>penalty</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$26,Tabelle1!$C$28,Tabelle1!$C$30:$C$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$G$26,Tabelle1!$G$28,Tabelle1!$G$30:$G$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.15140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2927E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3440000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7650999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4999000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.614E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Nitsche</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$45,Tabelle1!$C$47,Tabelle1!$C$49:$C$52)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$G$45,Tabelle1!$G$47,Tabelle1!$G$49:$G$52)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3119999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3974E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7743999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5856999999999998E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="102983552"/>
+        <c:axId val="102989824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="102983552"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102989824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="102989824"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102983552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Energy-norm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lagrange</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$6,Tabelle1!$C$8,Tabelle1!$C$10:$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$H$8,Tabelle1!$H$6,Tabelle1!$H$10:$H$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.28494000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27418999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28938000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29049000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29097000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29160000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>penalty</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$26,Tabelle1!$C$29,Tabelle1!$C$29,Tabelle1!$C$28,Tabelle1!$C$30:$C$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$H$26,Tabelle1!$H$28,Tabelle1!$H$30:$H$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.27483000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28494000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28938000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29049000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29097000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29160000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Nitsche</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$45,Tabelle1!$C$47,Tabelle1!$C$49:$C$52)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$H$45,Tabelle1!$H$48,Tabelle1!$H$48,Tabelle1!$H$47,Tabelle1!$H$49:$H$52)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.27421000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28494000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28938000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29049000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29097000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29160000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="69804032"/>
+        <c:axId val="69805568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69804032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69805568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69805568"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69804032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Traction-norm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lagrange</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$6,Tabelle1!$C$8,Tabelle1!$C$10,Tabelle1!$C$12,Tabelle1!$C$12,Tabelle1!$C$11:$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$I$6,Tabelle1!$I$8,Tabelle1!$I$10:$I$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.84238999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95969000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97304000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97970000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98975999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>penalty</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$26,Tabelle1!$C$28,Tabelle1!$C$30:$C$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$I$26,Tabelle1!$I$28,Tabelle1!$I$30:$I$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.4292000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6520000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4087000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4513999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6424999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4396E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Nitsche</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$C$45,Tabelle1!$C$47,Tabelle1!$C$49:$C$52)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.50619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3892000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Tabelle1!$I$45,Tabelle1!$I$47,Tabelle1!$I$49:$I$52)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.1199000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0854000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0261999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4504000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3596999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5272999999999997E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="69841664"/>
+        <c:axId val="69843200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69841664"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69843200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69843200"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69841664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1282,14 +2084,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162485</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:colOff>196103</xdr:colOff>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>93009</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2515160</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:colOff>2548778</xdr:colOff>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>169209</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1312,15 +2114,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>108137</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>119343</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1052234</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>184337</xdr:rowOff>
+      <xdr:colOff>1130675</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>5043</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1342,15 +2144,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1337423</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>121022</xdr:rowOff>
+      <xdr:colOff>1292599</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>64993</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>355787</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>6722</xdr:rowOff>
+      <xdr:colOff>310963</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>141193</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1364,6 +2166,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>224117</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>128869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2576792</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>14569</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>218514</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>155203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1158689</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>40903</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1320613</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>338977</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>177053</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1659,8 +2551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="C59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1674,6 +2566,7 @@
     <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1719,6 +2612,9 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
+      <c r="C6">
+        <v>0.50619999999999998</v>
+      </c>
       <c r="D6">
         <v>252</v>
       </c>
@@ -1745,6 +2641,9 @@
       <c r="K7" t="s">
         <v>12</v>
       </c>
+      <c r="L7">
+        <v>0.38624000000000003</v>
+      </c>
       <c r="M7">
         <v>492</v>
       </c>
@@ -1768,6 +2667,9 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
+      <c r="C8">
+        <v>0.27940999999999999</v>
+      </c>
       <c r="D8">
         <v>820</v>
       </c>
@@ -1791,6 +2693,9 @@
       <c r="K9" t="s">
         <v>9</v>
       </c>
+      <c r="L9">
+        <v>0.19373000000000001</v>
+      </c>
       <c r="M9">
         <v>1944</v>
       </c>
@@ -1814,6 +2719,9 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
+      <c r="C10">
+        <v>0.14055000000000001</v>
+      </c>
       <c r="D10">
         <v>3240</v>
       </c>
@@ -1837,6 +2745,9 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
+      <c r="C11">
+        <v>9.3892000000000003E-2</v>
+      </c>
       <c r="D11">
         <v>7260</v>
       </c>
@@ -1860,6 +2771,9 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
+      <c r="C12">
+        <v>7.0490999999999998E-2</v>
+      </c>
       <c r="D12">
         <v>12880</v>
       </c>
@@ -1882,6 +2796,9 @@
     <row r="13" spans="1:18">
       <c r="B13" t="s">
         <v>17</v>
+      </c>
+      <c r="C13">
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="D13">
         <v>51360</v>
@@ -2011,6 +2928,9 @@
       <c r="B26" t="s">
         <v>18</v>
       </c>
+      <c r="C26">
+        <v>0.50619999999999998</v>
+      </c>
       <c r="D26">
         <v>252</v>
       </c>
@@ -2037,6 +2957,9 @@
       <c r="K27" t="s">
         <v>12</v>
       </c>
+      <c r="L27">
+        <v>0.38624000000000003</v>
+      </c>
       <c r="M27">
         <v>492</v>
       </c>
@@ -2063,6 +2986,9 @@
       <c r="B28" t="s">
         <v>19</v>
       </c>
+      <c r="C28">
+        <v>0.27940999999999999</v>
+      </c>
       <c r="D28">
         <v>820</v>
       </c>
@@ -2115,6 +3041,9 @@
       <c r="B30" t="s">
         <v>13</v>
       </c>
+      <c r="C30">
+        <v>0.14055000000000001</v>
+      </c>
       <c r="D30">
         <v>3240</v>
       </c>
@@ -2141,6 +3070,9 @@
       <c r="B31" t="s">
         <v>15</v>
       </c>
+      <c r="C31">
+        <v>9.3892000000000003E-2</v>
+      </c>
       <c r="D31">
         <v>7260</v>
       </c>
@@ -2168,6 +3100,9 @@
       <c r="B32" t="s">
         <v>16</v>
       </c>
+      <c r="C32">
+        <v>7.0490999999999998E-2</v>
+      </c>
       <c r="D32">
         <v>12880</v>
       </c>
@@ -2193,6 +3128,9 @@
       </c>
       <c r="B33" t="s">
         <v>17</v>
+      </c>
+      <c r="C33">
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="D33">
         <v>51360</v>
@@ -2334,6 +3272,9 @@
       <c r="B45" t="s">
         <v>18</v>
       </c>
+      <c r="C45">
+        <v>0.50619999999999998</v>
+      </c>
       <c r="D45">
         <v>252</v>
       </c>
@@ -2360,6 +3301,9 @@
       <c r="K46" t="s">
         <v>12</v>
       </c>
+      <c r="L46">
+        <v>0.38624000000000003</v>
+      </c>
       <c r="M46">
         <v>492</v>
       </c>
@@ -2386,6 +3330,9 @@
       <c r="B47" t="s">
         <v>19</v>
       </c>
+      <c r="C47">
+        <v>0.27940999999999999</v>
+      </c>
       <c r="D47">
         <v>820</v>
       </c>
@@ -2438,6 +3385,9 @@
       <c r="B49" t="s">
         <v>13</v>
       </c>
+      <c r="C49">
+        <v>0.14055000000000001</v>
+      </c>
       <c r="D49">
         <v>3240</v>
       </c>
@@ -2464,6 +3414,9 @@
       <c r="B50" t="s">
         <v>15</v>
       </c>
+      <c r="C50">
+        <v>9.3892000000000003E-2</v>
+      </c>
       <c r="D50">
         <v>7260</v>
       </c>
@@ -2490,6 +3443,9 @@
       <c r="B51" t="s">
         <v>16</v>
       </c>
+      <c r="C51">
+        <v>7.0490999999999998E-2</v>
+      </c>
       <c r="D51">
         <v>12880</v>
       </c>
@@ -2515,6 +3471,9 @@
       </c>
       <c r="B52" t="s">
         <v>17</v>
+      </c>
+      <c r="C52">
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="D52">
         <v>51360</v>

</xml_diff>

<commit_message>
Perfect plasticity is implemented for penalty and Nitsche's method. The results seem to be good, but there is no proof via a comparison to an analytical solution, yet. The modifications of the Lagrange multiplier routines have begun, but it doesn't work, yet.
</commit_message>
<xml_diff>
--- a/error_computation/frictionless_sliding_analyt_8/database.xlsx
+++ b/error_computation/frictionless_sliding_analyt_8/database.xlsx
@@ -485,11 +485,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87243008"/>
-        <c:axId val="87248896"/>
+        <c:axId val="82917632"/>
+        <c:axId val="82927616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87243008"/>
+        <c:axId val="82917632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -497,12 +497,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87248896"/>
+        <c:crossAx val="82927616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87248896"/>
+        <c:axId val="82927616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -511,7 +511,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87243008"/>
+        <c:crossAx val="82917632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -524,7 +524,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -851,11 +851,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87498752"/>
-        <c:axId val="87500288"/>
+        <c:axId val="83103744"/>
+        <c:axId val="83105280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87498752"/>
+        <c:axId val="83103744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -863,12 +863,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87500288"/>
+        <c:crossAx val="83105280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87500288"/>
+        <c:axId val="83105280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -877,7 +877,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87498752"/>
+        <c:crossAx val="83103744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -890,7 +890,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1231,11 +1231,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87553152"/>
-        <c:axId val="87554688"/>
+        <c:axId val="83162240"/>
+        <c:axId val="83163776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87553152"/>
+        <c:axId val="83162240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1243,12 +1243,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87554688"/>
+        <c:crossAx val="83163776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87554688"/>
+        <c:axId val="83163776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1257,7 +1257,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87553152"/>
+        <c:crossAx val="83162240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1270,7 +1270,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1296,7 +1296,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1492,11 +1491,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102983552"/>
-        <c:axId val="102989824"/>
+        <c:axId val="83185664"/>
+        <c:axId val="83187200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102983552"/>
+        <c:axId val="83185664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1504,12 +1503,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102989824"/>
+        <c:crossAx val="83187200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102989824"/>
+        <c:axId val="83187200"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1518,14 +1517,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102983552"/>
+        <c:crossAx val="83185664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1753,11 +1751,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69804032"/>
-        <c:axId val="69805568"/>
+        <c:axId val="87624320"/>
+        <c:axId val="87626112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69804032"/>
+        <c:axId val="87624320"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1765,12 +1763,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69805568"/>
+        <c:crossAx val="87626112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69805568"/>
+        <c:axId val="87626112"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1779,7 +1777,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69804032"/>
+        <c:crossAx val="87624320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2034,11 +2032,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69841664"/>
-        <c:axId val="69843200"/>
+        <c:axId val="87664128"/>
+        <c:axId val="87665664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69841664"/>
+        <c:axId val="87664128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2046,12 +2044,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69843200"/>
+        <c:crossAx val="87665664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69843200"/>
+        <c:axId val="87665664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2060,7 +2058,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69841664"/>
+        <c:crossAx val="87664128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2551,8 +2549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:C52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>